<commit_message>
fix: Actualizacion de los formatos xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/templates_files/Resultados de admisión.xlsx
+++ b/src/main/resources/templates_files/Resultados de admisión.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sainos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C84A0-2A26-4F3E-8715-8BF47FD1A483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A12A1C-EECD-47E4-BBC7-9B101FB3266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{2E792FEF-85A4-44F9-8821-F1189C2311A1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Nombre completo</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>GRBH010228HOCNRLA7</t>
+  </si>
+  <si>
+    <t>Calificación</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -206,6 +209,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346EFF7E-3BFA-4838-8FF0-22ADDB6905E8}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +540,7 @@
     <col min="6" max="6" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -555,8 +559,11 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -572,8 +579,11 @@
       <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -589,8 +599,11 @@
       <c r="E3" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -609,8 +622,11 @@
       <c r="F4">
         <v>99.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -626,8 +642,11 @@
       <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -643,8 +662,11 @@
       <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -660,8 +682,11 @@
       <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -677,8 +702,11 @@
       <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -694,37 +722,40 @@
       <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>

</xml_diff>

<commit_message>
fix: se actualizo el xlss
</commit_message>
<xml_diff>
--- a/src/main/resources/templates_files/Resultados de admisión.xlsx
+++ b/src/main/resources/templates_files/Resultados de admisión.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sainos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C84A0-2A26-4F3E-8715-8BF47FD1A483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A12A1C-EECD-47E4-BBC7-9B101FB3266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{2E792FEF-85A4-44F9-8821-F1189C2311A1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Nombre completo</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>GRBH010228HOCNRLA7</t>
+  </si>
+  <si>
+    <t>Calificación</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -206,6 +209,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346EFF7E-3BFA-4838-8FF0-22ADDB6905E8}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +540,7 @@
     <col min="6" max="6" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -555,8 +559,11 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -572,8 +579,11 @@
       <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -589,8 +599,11 @@
       <c r="E3" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -609,8 +622,11 @@
       <c r="F4">
         <v>99.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -626,8 +642,11 @@
       <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -643,8 +662,11 @@
       <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -660,8 +682,11 @@
       <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -677,8 +702,11 @@
       <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -694,37 +722,40 @@
       <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>

</xml_diff>